<commit_message>
add atur jadwal create and db
</commit_message>
<xml_diff>
--- a/upload/format_nilai.xlsx
+++ b/upload/format_nilai.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\silusi\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9764056C-6A3A-4C7C-872C-C2DEE747718B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{471ADABB-9D47-43A1-9D3F-EA0973A0465F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0E717172-3C02-4D07-A468-817235BFE0E7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A82D7D7-8799-4CE0-9B40-A81B2BF49032}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,89 +36,80 @@
     <t>nomor_ujian</t>
   </si>
   <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>nilai_ujian_sekolah</t>
+  </si>
+  <si>
+    <t>nilai_usp</t>
+  </si>
+  <si>
+    <t>rerata</t>
+  </si>
+  <si>
     <t>2-18-19-20-0001</t>
   </si>
   <si>
+    <t>Ardha</t>
+  </si>
+  <si>
     <t>2-18-19-20-0002</t>
   </si>
   <si>
+    <t>Robby</t>
+  </si>
+  <si>
     <t>2-18-19-20-0003</t>
   </si>
   <si>
+    <t>Firmansyah</t>
+  </si>
+  <si>
     <t>2-18-19-20-0004</t>
   </si>
   <si>
+    <t>Firman</t>
+  </si>
+  <si>
     <t>2-18-19-20-0005</t>
   </si>
   <si>
+    <t>Agus</t>
+  </si>
+  <si>
     <t>2-18-19-20-0006</t>
   </si>
   <si>
+    <t>Atlas</t>
+  </si>
+  <si>
     <t>2-18-19-20-0007</t>
   </si>
   <si>
+    <t xml:space="preserve">Baret </t>
+  </si>
+  <si>
     <t>2-18-19-20-0008</t>
   </si>
   <si>
+    <t>Reneta</t>
+  </si>
+  <si>
     <t>2-18-19-20-0009</t>
   </si>
   <si>
-    <t>nama</t>
-  </si>
-  <si>
-    <t>Agus</t>
-  </si>
-  <si>
-    <t>Ardha</t>
-  </si>
-  <si>
-    <t>Robby</t>
-  </si>
-  <si>
-    <t>Firmansyah</t>
-  </si>
-  <si>
-    <t>Firman</t>
-  </si>
-  <si>
-    <t>Atlas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baret </t>
-  </si>
-  <si>
-    <t>Reneta</t>
-  </si>
-  <si>
     <t>Asmin</t>
-  </si>
-  <si>
-    <t>nilai ujian sekolah</t>
-  </si>
-  <si>
-    <t>nilai usp</t>
-  </si>
-  <si>
-    <t>rata rata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,9 +135,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,22 +450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B4EF20-18D4-4820-8FEB-F5440C998BE4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6152E11A-BB69-4A6A-85B6-A31D88BCA285}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,19 +473,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -506,23 +493,23 @@
         <v>7888</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="G2">
         <f>AVERAGE(E2:F2)</f>
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -530,23 +517,23 @@
         <v>7889</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>95</v>
       </c>
       <c r="F3">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G10" si="0">AVERAGE(E3:F3)</f>
-        <v>86.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -554,23 +541,23 @@
         <v>7890</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>79</v>
       </c>
       <c r="F4">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>84.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -578,23 +565,23 @@
         <v>7891</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>77</v>
       </c>
       <c r="F5">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>82.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -602,23 +589,23 @@
         <v>7892</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>74</v>
       </c>
       <c r="F6">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -626,7 +613,7 @@
         <v>7893</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -635,14 +622,14 @@
         <v>71</v>
       </c>
       <c r="F7">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -650,23 +637,23 @@
         <v>7894</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>78</v>
       </c>
       <c r="F8">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>80.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -674,23 +661,23 @@
         <v>7895</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>90</v>
       </c>
       <c r="F9">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G9">
-        <f>AVERAGE(E9:F9)</f>
-        <v>86.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -698,25 +685,23 @@
         <v>7896</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>88</v>
       </c>
       <c r="F10">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G10">
-        <f>AVERAGE(E10:F10)</f>
-        <v>85.5</v>
+        <f t="shared" si="0"/>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>